<commit_message>
Update thesis files, add appendices, and clean outputs
Added .github/copilot-instructions.md for project guidance. Updated .gitignore to exclude generated analysis outputs and caches. Substantially revised FINAL_INTEGRATED_REPORT.tex with new findings, robustness checks, and improved figure path handling. Enhanced README.md with clearer analysis instructions and data structure. Improved Thesis writing for template fallback, Unicode, and finalized abstract. Added appendix files for instruments, materials, and stats. Removed obsolete R history and generated plot/table outputs from version control.
</commit_message>
<xml_diff>
--- a/final_analysis/AI*memory results.xlsx
+++ b/final_analysis/AI*memory results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duccioo/Desktop/ai_memory_experiment/final_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7993A85-3553-7D42-BD8C-A760A1E9C0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C610151-7CD3-B64E-823D-882BFCB89C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="760" windowWidth="25280" windowHeight="17400" xr2:uid="{FD95DE68-70A6-2A40-8D0A-73722392BCD1}"/>
+    <workbookView xWindow="3300" yWindow="760" windowWidth="25280" windowHeight="17400" activeTab="2" xr2:uid="{FD95DE68-70A6-2A40-8D0A-73722392BCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="MCQ" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,19 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E7DD34A1-2E08-534D-AF7D-DA66518B45CC}</author>
+    <author>tc={F215F4F4-7FEA-A149-86D1-2B9B30D07DD4}</author>
   </authors>
   <commentList>
     <comment ref="C6" authorId="0" shapeId="0" xr:uid="{E7DD34A1-2E08-534D-AF7D-DA66518B45CC}">
+      <text>
+        <t xml:space="preserve">[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+For this I calculated I divided the reading time by the summary time as it was considered all together
+</t>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="1" shapeId="0" xr:uid="{F215F4F4-7FEA-A149-86D1-2B9B30D07DD4}">
       <text>
         <t xml:space="preserve">[Commento in thread]
 La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
@@ -57,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="133">
   <si>
     <t>synchronous</t>
   </si>
@@ -110,28 +120,16 @@
     <t>average for non AI:8.26</t>
   </si>
   <si>
-    <t>average for with AI:18.71</t>
-  </si>
-  <si>
     <t>5.92</t>
   </si>
   <si>
     <t>6.00</t>
   </si>
   <si>
-    <t>6.18 </t>
-  </si>
-  <si>
-    <t>5.72</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.25 </t>
   </si>
   <si>
     <t>5.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average for integrated: 6.03 </t>
   </si>
   <si>
     <t>average for segmented: 5.56</t>
@@ -310,43 +308,10 @@
 For subjective ratings (mental effort, task difficulty, and MCQ confidence), all values fall within the expected 1–7 scale. One AI participant (P235) is missing one post-article rating entry, resulting in reduced n for rating-based analyses involving that article only. No duplicate rating submissions were detected.</t>
   </si>
   <si>
-    <t>AI trust: 4.94/7</t>
-  </si>
-  <si>
-    <t>AI dependence 5.15/7</t>
-  </si>
-  <si>
     <t xml:space="preserve"> For the AI conditions (integrated and segmented), duplicate recall submissions were observed for a subset of participants (P240, P246, P251, P253, P258, P263, P264, and P266). In these cases, the duplicate entries contained identical recall text, suggesting that the duplicates likely resulted from double submission or transient network issues rather than substantive changes to responses.
 In the No-AI condition, duplicate recall submissions with identical content were observed for P186 and P188.
 All duplicate cases were resolved using a predefined deduplication rule, retaining the last submission per participant × article (and per phase for AI) based on timestamp.
 Recall scoring was applied only to retained recall responses. All retained recall records contain complete textual responses and valid scoring fields.</t>
-  </si>
-  <si>
-    <t>27.49%</t>
-  </si>
-  <si>
-    <t>16.85%</t>
-  </si>
-  <si>
-    <t>15.44%</t>
-  </si>
-  <si>
-    <t>24.38%</t>
-  </si>
-  <si>
-    <t>14.43%</t>
-  </si>
-  <si>
-    <t>13.38%</t>
-  </si>
-  <si>
-    <t>average for segmented:17.40%</t>
-  </si>
-  <si>
-    <t>summary reading time percentage: ai_summary reading time/overall reading time (%) 20.07%</t>
-  </si>
-  <si>
-    <t>average for integrated: 20.07%</t>
   </si>
   <si>
     <t>average for with AI:0.4653</t>
@@ -382,21 +347,6 @@
   </si>
   <si>
     <t>average for non AI:5.403</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6.44</t>
-  </si>
-  <si>
-    <t>6.76</t>
-  </si>
-  <si>
-    <t>average for integrated:7.25</t>
-  </si>
-  <si>
-    <t>average for segmented: 6.76</t>
-  </si>
-  <si>
-    <t>average for with AI:7.01</t>
   </si>
   <si>
     <t>reading time: overall 7.43</t>
@@ -514,18 +464,6 @@
     <t>mental effort: overall</t>
   </si>
   <si>
-    <t>Integrated:5.17</t>
-  </si>
-  <si>
-    <t>Integrated:5.00</t>
-  </si>
-  <si>
-    <t>segmented: 5.31</t>
-  </si>
-  <si>
-    <t>segmented: 4.72</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -558,12 +496,120 @@
 So, integrated participants report higher trust but slightly lower dependence than segmented.</t>
     </r>
   </si>
+  <si>
+    <t>7.45</t>
+  </si>
+  <si>
+    <t>6.93</t>
+  </si>
+  <si>
+    <t>average for integrated:7.59</t>
+  </si>
+  <si>
+    <t>average for segmented: 6.81</t>
+  </si>
+  <si>
+    <t>average for with AI:7.20</t>
+  </si>
+  <si>
+    <t>average for integrated: 6.00</t>
+  </si>
+  <si>
+    <t>24.37%</t>
+  </si>
+  <si>
+    <t>18.24%</t>
+  </si>
+  <si>
+    <t>13.45%</t>
+  </si>
+  <si>
+    <t>25.15%</t>
+  </si>
+  <si>
+    <t>19.54%</t>
+  </si>
+  <si>
+    <t>12.70%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">summary reading time percentage: ai_summary reading time/overall reading time (%) </t>
+  </si>
+  <si>
+    <t>4.17</t>
+  </si>
+  <si>
+    <t>3.58</t>
+  </si>
+  <si>
+    <t>3.92</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>4.83</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI trust: </t>
+  </si>
+  <si>
+    <t>average for integrated:3.89</t>
+  </si>
+  <si>
+    <t>average for segmented: 4.33</t>
+  </si>
+  <si>
+    <t>average for with AI:4.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI dependence </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.83 </t>
+  </si>
+  <si>
+    <t>3.67</t>
+  </si>
+  <si>
+    <t>5.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.58</t>
+  </si>
+  <si>
+    <t>average for integrated:3.92</t>
+  </si>
+  <si>
+    <t>average for segmented: 4.81</t>
+  </si>
+  <si>
+    <t>average for with AI:4.36</t>
+  </si>
+  <si>
+    <t>average for integrated: 18.69%</t>
+  </si>
+  <si>
+    <t>average for segmented:19.13%</t>
+  </si>
+  <si>
+    <t>average for with AI:18.91%</t>
+  </si>
+  <si>
+    <t>6.18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -605,8 +651,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,14 +677,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -738,24 +784,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -782,8 +815,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -830,12 +862,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1174,6 +1200,10 @@
     <text xml:space="preserve">For this I calculated I divided the reading time by the summary time as it was considered all together
 </text>
   </threadedComment>
+  <threadedComment ref="C30" dT="2025-12-23T18:21:04.52" personId="{B477FAF7-47F2-0E41-8BBC-3E42CA450F9C}" id="{F215F4F4-7FEA-A149-86D1-2B9B30D07DD4}">
+    <text xml:space="preserve">For this I calculated I divided the reading time by the summary time as it was considered all together
+</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1181,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA31AC7-00DF-2444-8B96-2059A82A4B9E}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1197,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,7 +1237,7 @@
     </row>
     <row r="3" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -1218,34 +1248,34 @@
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="J5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1273,52 +1303,52 @@
     </row>
     <row r="7" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="19" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1328,26 +1358,26 @@
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
@@ -1371,49 +1401,49 @@
     </row>
     <row r="15" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="G15" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="B17" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1423,26 +1453,26 @@
       <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
@@ -1466,49 +1496,49 @@
     </row>
     <row r="23" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="24" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
+      <c r="B25" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="27" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1518,26 +1548,26 @@
       <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24" t="s">
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
@@ -1561,49 +1591,49 @@
     </row>
     <row r="31" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="E31" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="B32" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
+      <c r="B33" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1613,26 +1643,26 @@
       <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24" t="s">
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="17" t="s">
@@ -1656,45 +1686,45 @@
     </row>
     <row r="39" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="G39" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="40" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="B40" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
+      <c r="B41" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -1749,7 +1779,7 @@
     <row r="1" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1760,29 +1790,29 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1826,33 +1856,33 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="B8" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
+      <c r="B9" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1863,29 +1893,29 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="34" t="s">
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
@@ -1909,47 +1939,47 @@
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="G16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="3" t="s">
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="3" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -1957,7 +1987,7 @@
         <v>7</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
@@ -1971,7 +2001,7 @@
         <v>9</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -1986,7 +2016,7 @@
     </row>
     <row r="27" spans="2:14" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N27" s="12" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2012,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37130725-7234-5948-A62B-4813CD0B44B0}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:G36"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2026,12 +2056,12 @@
         <v>7</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2045,29 +2075,29 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
       <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -2092,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2100,7 +2130,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>13</v>
@@ -2109,7 +2139,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>15</v>
@@ -2119,33 +2149,33 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33" t="s">
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2155,26 +2185,26 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -2199,49 +2229,49 @@
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="10" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="B15" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="B16" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2251,53 +2281,91 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41" t="s">
+      <c r="B20" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2307,60 +2375,90 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
+      <c r="B28" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
+      <c r="B31" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
+      <c r="B32" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -2372,30 +2470,30 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="42" t="s">
+      <c r="C36" s="40"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -2423,55 +2521,56 @@
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="D38" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="B39" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="38"/>
-      <c r="G39" s="45"/>
+      <c r="B39" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="37"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="37"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="B40" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
+      <c r="B40" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
       <c r="H40" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
@@ -2487,6 +2586,7 @@
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:D4"/>
@@ -2523,7 +2623,7 @@
     <row r="1" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="3:3" ht="206" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="12" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>